<commit_message>
v0.0.2alpha: Create comments based on excel data
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\College\Florida Southern College\Extra Files\Lakeland Regional\Research\AsanaAPISync\AsanaAPISync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855af64d26289e3e/College/Florida Southern College/Extra Files/Lakeland Regional/Research/AsanaAPISync/AsanaAPISync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F84F1D97-9045-4471-B81D-5228464F8AA5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Project</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Back Pain in ED</t>
   </si>
   <si>
-    <t>AsanaAPISync_v0.0.2alpha: Document parsing test 1</t>
-  </si>
-  <si>
     <t>AsanaAPISync_v0.0.2alpha: Document parsing test 4</t>
   </si>
   <si>
@@ -98,6 +95,12 @@
   </si>
   <si>
     <t>AsanaAPISync_v0.0.2alpha: Document parsing test 3</t>
+  </si>
+  <si>
+    <t>AsanaAPISync_v0.0.2alpha: Dynamic fetching test 2</t>
+  </si>
+  <si>
+    <t>Meeting: Intake</t>
   </si>
 </sst>
 </file>
@@ -540,13 +543,14 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -580,13 +584,13 @@
         <v>45594</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>8.1999999999999993</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -606,7 +610,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -626,7 +630,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -646,7 +650,7 @@
         <v>11.2</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.0.0: Published first release as npm package
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855af64d26289e3e/College/Florida Southern College/Extra Files/Lakeland Regional/Research/AsanaAPISync/AsanaAPISync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F84F1D97-9045-4471-B81D-5228464F8AA5}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24BC04F5-EE11-4A6A-B916-46E10F79E982}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetA" sheetId="1" r:id="rId1"/>
     <sheet name="SheetB" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -49,6 +60,9 @@
     <t>bob</t>
   </si>
   <si>
+    <t>Drew1</t>
+  </si>
+  <si>
     <t>Tasky things</t>
   </si>
   <si>
@@ -58,56 +72,53 @@
     <t>jack</t>
   </si>
   <si>
+    <t>Drew2</t>
+  </si>
+  <si>
+    <t>This is jack's comment</t>
+  </si>
+  <si>
     <t>henry</t>
   </si>
   <si>
+    <t>Drew3</t>
+  </si>
+  <si>
+    <t>This is henry's comment</t>
+  </si>
+  <si>
     <t>jim</t>
   </si>
   <si>
+    <t>Drew4</t>
+  </si>
+  <si>
     <t>This is jim's comment</t>
   </si>
   <si>
-    <t>This is henry's comment</t>
-  </si>
-  <si>
-    <t>This is jack's comment</t>
-  </si>
-  <si>
-    <t>Drew1</t>
-  </si>
-  <si>
-    <t>Drew2</t>
-  </si>
-  <si>
-    <t>Drew3</t>
-  </si>
-  <si>
-    <t>Drew4</t>
-  </si>
-  <si>
     <t>Back Pain in ED</t>
   </si>
   <si>
+    <t>Meeting: Intake</t>
+  </si>
+  <si>
+    <t>AsanaAPISync_v0.0.2alpha: Dynamic fetching test 2</t>
+  </si>
+  <si>
+    <t>AsanaAPISync_v0.0.2alpha: Document parsing test 2</t>
+  </si>
+  <si>
+    <t>AsanaAPISync_v0.0.2alpha: Document parsing test 3</t>
+  </si>
+  <si>
     <t>AsanaAPISync_v0.0.2alpha: Document parsing test 4</t>
-  </si>
-  <si>
-    <t>AsanaAPISync_v0.0.2alpha: Document parsing test 2</t>
-  </si>
-  <si>
-    <t>AsanaAPISync_v0.0.2alpha: Document parsing test 3</t>
-  </si>
-  <si>
-    <t>AsanaAPISync_v0.0.2alpha: Dynamic fetching test 2</t>
-  </si>
-  <si>
-    <t>Meeting: Intake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +428,31 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{D62FE5AD-153E-41FD-8C82-57D521732131}">
+  <we:reference id="WA104099688" version="1.7.0.0" store="en-US" storeType="omex"/>
+  <we:alternateReferences>
+    <we:reference id="WA104099688" version="1.7.0.0" store="omex" storeType="omex"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
@@ -425,14 +461,14 @@
       <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,84 +488,84 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>45594</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>8.1999999999999993</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>45595</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>9.1999999999999993</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>45595</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>10.199999999999999</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>45595</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>11.2</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -546,14 +582,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,84 +609,84 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>45594</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>8.1999999999999993</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>45595</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>9.1999999999999993</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>45595</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>10.199999999999999</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>45595</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>11.2</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed whitespace and date bugs
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855af64d26289e3e/College/Florida Southern College/Extra Files/Lakeland Regional/Research/AsanaAPISync/AsanaAPISync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855af64d26289e3e/Lakeland Regional/Research/AsanaAPISync/AsanaAPISync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24BC04F5-EE11-4A6A-B916-46E10F79E982}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{02A2D4DC-BFE5-48F1-9E4F-B0DBADBFCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A9C9219-8022-416E-877E-FEDC8328E585}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,9 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,14 +462,14 @@
       <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -508,7 +509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -528,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -548,7 +549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -579,17 +580,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -629,7 +630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -649,7 +650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -669,14 +670,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>45595</v>
       </c>
       <c r="D5" t="s">

</xml_diff>